<commit_message>
mise a jour de la navigation
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>Description</t>
   </si>
@@ -203,14 +203,38 @@
     <t>Romain Sire</t>
   </si>
   <si>
-    <t xml:space="preserve">Recherche des entreprises qui </t>
+    <t>Recherche des entreprises qui ont déjà pris des stagiaires</t>
+  </si>
+  <si>
+    <t>EntrepriseController</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ListeEntreprise </t>
+  </si>
+  <si>
+    <t>Collaborateur</t>
+  </si>
+  <si>
+    <t>Liste des entreprises pour modification/creation,suppression</t>
+  </si>
+  <si>
+    <t>ListeEntreprisePourModification</t>
+  </si>
+  <si>
+    <t>Saisie autorisation d'absence</t>
+  </si>
+  <si>
+    <t>AutorisationAbsenceController</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CompleterInfoAbsence </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +265,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -262,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -272,6 +303,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,15 +584,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="243.7109375" bestFit="1" customWidth="1"/>
@@ -746,12 +779,46 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="15.75">
       <c r="A21" t="s">
         <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>39</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit navigation presque fini au niveau admin et collaborateur
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -170,9 +170,6 @@
     <t>Florian Peyramard</t>
   </si>
   <si>
-    <t>Affichage liste satagiaire</t>
-  </si>
-  <si>
     <t>OffredeFormationBeneficiaire</t>
   </si>
   <si>
@@ -249,6 +246,9 @@
   </si>
   <si>
     <t>ListePeeAValider</t>
+  </si>
+  <si>
+    <t>Affichage liste benificiaire</t>
   </si>
 </sst>
 </file>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -755,16 +755,16 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
         <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -772,60 +772,60 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>36</v>
-      </c>
-      <c r="D19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75">
       <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
         <v>42</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75">
@@ -833,51 +833,51 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="B24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="D25" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="B26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" t="s">
         <v>53</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modification pour intégration tristan
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t xml:space="preserve">Droit</t>
   </si>
@@ -286,13 +286,16 @@
     <t xml:space="preserve">FileUpload</t>
   </si>
   <si>
+    <t xml:space="preserve">Adm/Collaborateur</t>
+  </si>
+  <si>
     <t xml:space="preserve">Affichage de l’annuaire social</t>
   </si>
   <si>
     <t xml:space="preserve">AnnuaireSocial/GestionAnnuaire</t>
   </si>
   <si>
-    <t xml:space="preserve">Adm/Collaborateur</t>
+    <t xml:space="preserve">LigneAnnuaires</t>
   </si>
   <si>
     <t xml:space="preserve">Affichage des catégories pour la gestion Annuaire</t>
@@ -320,7 +323,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -378,12 +381,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -427,7 +424,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -445,14 +442,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,15 +533,15 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="243.71"/>
   </cols>
   <sheetData>
@@ -833,58 +826,58 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D31" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D32" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D33" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>